<commit_message>
Add URLs to videos
</commit_message>
<xml_diff>
--- a/AFP_Group2/Resources/Misconceptions.xlsx
+++ b/AFP_Group2/Resources/Misconceptions.xlsx
@@ -10,8 +10,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A6">
+      <text>
+        <t xml:space="preserve">han looking for the video
+	-Manuela Peñuela</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
   <si>
     <t>Misconception</t>
   </si>
@@ -37,6 +53,9 @@
     <t>HighlightColor</t>
   </si>
   <si>
+    <t>VideoLink</t>
+  </si>
+  <si>
     <t>IT Careers are not creative</t>
   </si>
   <si>
@@ -61,6 +80,9 @@
     <t>redish</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/r1rcb2fh.mov</t>
+  </si>
+  <si>
     <t>Men are better than women in sciences</t>
   </si>
   <si>
@@ -79,6 +101,9 @@
     <t>video2</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/bxs5vxop.mov</t>
+  </si>
+  <si>
     <t>Women often fail in IT careers</t>
   </si>
   <si>
@@ -94,6 +119,9 @@
     <t>video3</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/jfb31hc4.mov</t>
+  </si>
+  <si>
     <t>Women aren't smart enough for a career in IT</t>
   </si>
   <si>
@@ -112,6 +140,9 @@
     <t>video4</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/t56jw9v.mov</t>
+  </si>
+  <si>
     <t>Women aren't good at coding</t>
   </si>
   <si>
@@ -130,6 +161,9 @@
     <t>video5</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/qd09o93s.mov</t>
+  </si>
+  <si>
     <t>Women aren't likely to get leadership in the IT industry</t>
   </si>
   <si>
@@ -148,6 +182,9 @@
     <t>video6</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/ypyvkg83.mov</t>
+  </si>
+  <si>
     <t>Most people that work in IT are male</t>
   </si>
   <si>
@@ -163,6 +200,9 @@
     <t>video7</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/vd1n9b52.mov</t>
+  </si>
+  <si>
     <t>Women aren't taken seriously in the IT industry</t>
   </si>
   <si>
@@ -181,6 +221,9 @@
     <t>video8</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/3aet286y.mov</t>
+  </si>
+  <si>
     <t>Workplace culture can feel excluding for women</t>
   </si>
   <si>
@@ -196,6 +239,9 @@
     <t>video9</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/p37bwlb6.mov</t>
+  </si>
+  <si>
     <t>Women get less opportunities than men</t>
   </si>
   <si>
@@ -208,6 +254,9 @@
     <t>video10</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/hywn16em.mov</t>
+  </si>
+  <si>
     <t>There aren't many female role models in the IT industry</t>
   </si>
   <si>
@@ -226,6 +275,9 @@
     <t>video11</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/jsbxi9h.mov</t>
+  </si>
+  <si>
     <t>Women are not good at IT</t>
   </si>
   <si>
@@ -244,7 +296,10 @@
     <t>video12</t>
   </si>
   <si>
-    <t>Women are held up to different standards than men</t>
+    <t>https://pomf2.lain.la/f/6dzw75oc.mov</t>
+  </si>
+  <si>
+    <t>IT is more challenging for women</t>
   </si>
   <si>
     <t>“It’s so easy for us to get caught up in negative patterns, versus seeing what positive change you can make. Especially for women and minorities, we need to learn to see challenges as stepping stones instead of hurdles. They really can bring you experience and closer to your goals.”</t>
@@ -262,6 +317,9 @@
     <t>video13</t>
   </si>
   <si>
+    <t>https://pomf2.lain.la/f/j33v6927.mov</t>
+  </si>
+  <si>
     <t>Women frequently experience being interrupted or talked over in professional settings</t>
   </si>
   <si>
@@ -278,13 +336,16 @@
   </si>
   <si>
     <t>video14</t>
+  </si>
+  <si>
+    <t>https://pomf2.lain.la/f/kjmpcmoy.mov</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -310,16 +371,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF5C5C5C"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF5C5C5C"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF5C5C5C"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F7F7"/>
+        <bgColor rgb="FFF7F7F7"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -340,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -350,16 +440,31 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -617,399 +722,461 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>15</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>15</v>
+        <v>58</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>15</v>
+        <v>65</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>15</v>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>15</v>
+        <v>83</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>15</v>
+        <v>90</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>15</v>
+        <v>97</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
+      <c r="A16" s="13"/>
     </row>
     <row r="17">
-      <c r="A17" s="8"/>
+      <c r="A17" s="13"/>
     </row>
     <row r="18">
-      <c r="A18" s="8"/>
+      <c r="A18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="8"/>
+      <c r="A19" s="13"/>
     </row>
     <row r="20">
-      <c r="A20" s="8"/>
+      <c r="A20" s="13"/>
     </row>
     <row r="21">
-      <c r="A21" s="8"/>
+      <c r="A21" s="13"/>
     </row>
     <row r="22">
-      <c r="A22" s="8"/>
+      <c r="A22" s="13"/>
     </row>
     <row r="23">
-      <c r="A23" s="8"/>
+      <c r="A23" s="13"/>
     </row>
     <row r="24">
-      <c r="A24" s="8"/>
+      <c r="A24" s="13"/>
     </row>
     <row r="25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="13"/>
     </row>
     <row r="26">
-      <c r="A26" s="8"/>
+      <c r="A26" s="13"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="I2"/>
+    <hyperlink r:id="rId3" ref="I3"/>
+    <hyperlink r:id="rId4" ref="I4"/>
+    <hyperlink r:id="rId5" ref="I5"/>
+    <hyperlink r:id="rId6" ref="I6"/>
+    <hyperlink r:id="rId7" ref="I7"/>
+    <hyperlink r:id="rId8" ref="I8"/>
+    <hyperlink r:id="rId9" ref="I9"/>
+    <hyperlink r:id="rId10" ref="I10"/>
+    <hyperlink r:id="rId11" ref="I11"/>
+    <hyperlink r:id="rId12" ref="I12"/>
+    <hyperlink r:id="rId13" ref="I13"/>
+    <hyperlink r:id="rId14" ref="I14"/>
+    <hyperlink r:id="rId15" ref="I15"/>
+  </hyperlinks>
+  <drawing r:id="rId16"/>
+  <legacyDrawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>